<commit_message>
Update a_psat forms, data files
</commit_message>
<xml_diff>
--- a/a_psat/data/answer_official.xlsx
+++ b/a_psat/data/answer_official.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\paedison3\a_psat\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_psat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106C1123-DF73-46D6-969D-759F12A6BB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BFDF4A-F2D7-4CEA-8D78-F8CD9ED00F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-54720" yWindow="2220" windowWidth="16440" windowHeight="28440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="정답" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +89,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -147,8 +153,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,14 +629,13 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.25" style="1" customWidth="1"/>
     <col min="2" max="5" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -655,16 +660,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -678,10 +683,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -692,13 +697,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -706,33 +711,33 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -740,16 +745,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3">
         <v>3</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -757,16 +762,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
         <v>2</v>
       </c>
       <c r="D8" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -774,13 +779,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3">
         <v>5</v>
@@ -791,16 +796,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" s="3">
         <v>5</v>
       </c>
       <c r="D10" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -817,7 +822,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -825,16 +830,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -842,16 +847,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -859,16 +864,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="7">
+        <v>4</v>
       </c>
       <c r="D14" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E14" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -879,13 +884,13 @@
         <v>3</v>
       </c>
       <c r="C15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
       </c>
       <c r="E15" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -893,16 +898,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16" s="3">
-        <v>4</v>
-      </c>
-      <c r="E16" s="3">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -910,16 +915,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D17" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -927,16 +932,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -944,16 +949,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="3">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E19" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -964,13 +969,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -978,13 +983,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="3">
         <v>3</v>
@@ -1001,7 +1006,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3">
         <v>3</v>
@@ -1012,13 +1017,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D23" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="3">
         <v>5</v>
@@ -1029,13 +1034,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C24" s="3">
         <v>4</v>
       </c>
       <c r="D24" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -1046,16 +1051,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D25" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E25" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1063,16 +1068,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="3">
         <v>2</v>
       </c>
       <c r="D26" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1081,13 +1086,13 @@
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D27" s="3">
         <v>5</v>
       </c>
       <c r="E27" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1096,10 +1101,10 @@
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
@@ -1111,13 +1116,13 @@
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="3">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
       </c>
       <c r="E29" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1126,13 +1131,13 @@
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D30" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1143,8 +1148,8 @@
       <c r="C31" s="3">
         <v>3</v>
       </c>
-      <c r="D31" s="3">
-        <v>2</v>
+      <c r="D31" s="7">
+        <v>5</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
@@ -1159,9 +1164,9 @@
         <v>3</v>
       </c>
       <c r="D32" s="3">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7">
         <v>4</v>
       </c>
     </row>
@@ -1171,10 +1176,10 @@
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="3">
-        <v>5</v>
-      </c>
-      <c r="D33" s="3">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D33" s="7">
+        <v>5</v>
       </c>
       <c r="E33" s="3">
         <v>4</v>
@@ -1188,11 +1193,11 @@
       <c r="C34" s="3">
         <v>3</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="7">
         <v>4</v>
       </c>
       <c r="E34" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1201,13 +1206,13 @@
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D35" s="3">
-        <v>4</v>
-      </c>
-      <c r="E35" s="3">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="E35" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1216,13 +1221,13 @@
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="3">
-        <v>1</v>
-      </c>
-      <c r="E36" s="3">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="E36" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1231,10 +1236,10 @@
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -1246,13 +1251,13 @@
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="3">
-        <v>1</v>
-      </c>
-      <c r="D38" s="3">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D38" s="7">
+        <v>2</v>
       </c>
       <c r="E38" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1261,13 +1266,13 @@
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="3">
-        <v>4</v>
-      </c>
-      <c r="D39" s="3">
-        <v>2</v>
-      </c>
-      <c r="E39" s="3">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D39" s="7">
+        <v>5</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1276,13 +1281,13 @@
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="3">
-        <v>5</v>
-      </c>
-      <c r="D40" s="3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D40" s="7">
+        <v>2</v>
       </c>
       <c r="E40" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1291,13 +1296,13 @@
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E41" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug in predict_utils (get_stat_data)
</commit_message>
<xml_diff>
--- a/a_psat/data/answer_official.xlsx
+++ b/a_psat/data/answer_official.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_psat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BFDF4A-F2D7-4CEA-8D78-F8CD9ED00F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3E5725-2294-46AC-B851-64955CBC5E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54720" yWindow="2220" windowWidth="16440" windowHeight="28440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27525" yWindow="9270" windowWidth="19080" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="정답" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -155,6 +155,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -626,9 +632,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -727,7 +733,7 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <v>3</v>
       </c>
       <c r="C6" s="3">
@@ -832,8 +838,8 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="3">
-        <v>1</v>
+      <c r="C12" s="7">
+        <v>3</v>
       </c>
       <c r="D12" s="3">
         <v>2</v>
@@ -889,7 +895,7 @@
       <c r="D15" s="3">
         <v>1</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="8">
         <v>4</v>
       </c>
     </row>
@@ -906,7 +912,7 @@
       <c r="D16" s="3">
         <v>1</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="8">
         <v>1</v>
       </c>
     </row>
@@ -923,7 +929,7 @@
       <c r="D17" s="3">
         <v>4</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="8">
         <v>4</v>
       </c>
     </row>
@@ -940,7 +946,7 @@
       <c r="D18" s="3">
         <v>4</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="8">
         <v>3</v>
       </c>
     </row>
@@ -957,7 +963,7 @@
       <c r="D19" s="3">
         <v>1</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="8">
         <v>2</v>
       </c>
     </row>
@@ -974,7 +980,7 @@
       <c r="D20" s="3">
         <v>3</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="8">
         <v>2</v>
       </c>
     </row>
@@ -991,7 +997,7 @@
       <c r="D21" s="3">
         <v>4</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1005,10 +1011,10 @@
       <c r="C22" s="3">
         <v>2</v>
       </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="D22" s="7">
+        <v>4</v>
+      </c>
+      <c r="E22" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1025,7 +1031,7 @@
       <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="8">
         <v>5</v>
       </c>
     </row>
@@ -1042,7 +1048,7 @@
       <c r="D24" s="3">
         <v>2</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1059,7 +1065,7 @@
       <c r="D25" s="3">
         <v>5</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1076,7 +1082,7 @@
       <c r="D26" s="3">
         <v>3</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="8">
         <v>5</v>
       </c>
     </row>
@@ -1091,7 +1097,7 @@
       <c r="D27" s="3">
         <v>5</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1106,7 +1112,7 @@
       <c r="D28" s="3">
         <v>2</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1118,10 +1124,10 @@
       <c r="C29" s="3">
         <v>3</v>
       </c>
-      <c r="D29" s="7">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3">
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8">
         <v>4</v>
       </c>
     </row>
@@ -1133,10 +1139,10 @@
       <c r="C30" s="3">
         <v>5</v>
       </c>
-      <c r="D30" s="3">
-        <v>3</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="D30" s="8">
+        <v>3</v>
+      </c>
+      <c r="E30" s="8">
         <v>4</v>
       </c>
     </row>
@@ -1148,10 +1154,10 @@
       <c r="C31" s="3">
         <v>3</v>
       </c>
-      <c r="D31" s="7">
-        <v>5</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="D31" s="8">
+        <v>5</v>
+      </c>
+      <c r="E31" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1163,10 +1169,10 @@
       <c r="C32" s="3">
         <v>3</v>
       </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" s="7">
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8">
         <v>4</v>
       </c>
     </row>
@@ -1178,10 +1184,10 @@
       <c r="C33" s="3">
         <v>1</v>
       </c>
-      <c r="D33" s="7">
-        <v>5</v>
-      </c>
-      <c r="E33" s="3">
+      <c r="D33" s="8">
+        <v>5</v>
+      </c>
+      <c r="E33" s="8">
         <v>4</v>
       </c>
     </row>
@@ -1193,10 +1199,10 @@
       <c r="C34" s="3">
         <v>3</v>
       </c>
-      <c r="D34" s="7">
-        <v>4</v>
-      </c>
-      <c r="E34" s="3">
+      <c r="D34" s="8">
+        <v>4</v>
+      </c>
+      <c r="E34" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1208,10 +1214,10 @@
       <c r="C35" s="3">
         <v>5</v>
       </c>
-      <c r="D35" s="3">
-        <v>2</v>
-      </c>
-      <c r="E35" s="7">
+      <c r="D35" s="8">
+        <v>2</v>
+      </c>
+      <c r="E35" s="8">
         <v>5</v>
       </c>
     </row>
@@ -1223,10 +1229,10 @@
       <c r="C36" s="3">
         <v>2</v>
       </c>
-      <c r="D36" s="3">
-        <v>3</v>
-      </c>
-      <c r="E36" s="7">
+      <c r="D36" s="8">
+        <v>3</v>
+      </c>
+      <c r="E36" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1238,10 +1244,10 @@
       <c r="C37" s="3">
         <v>4</v>
       </c>
-      <c r="D37" s="3">
-        <v>1</v>
-      </c>
-      <c r="E37" s="3">
+      <c r="D37" s="8">
+        <v>1</v>
+      </c>
+      <c r="E37" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1253,10 +1259,10 @@
       <c r="C38" s="3">
         <v>3</v>
       </c>
-      <c r="D38" s="7">
-        <v>2</v>
-      </c>
-      <c r="E38" s="3">
+      <c r="D38" s="8">
+        <v>2</v>
+      </c>
+      <c r="E38" s="8">
         <v>3</v>
       </c>
     </row>
@@ -1268,10 +1274,10 @@
       <c r="C39" s="3">
         <v>3</v>
       </c>
-      <c r="D39" s="7">
-        <v>5</v>
-      </c>
-      <c r="E39" s="7">
+      <c r="D39" s="8">
+        <v>5</v>
+      </c>
+      <c r="E39" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1283,10 +1289,10 @@
       <c r="C40" s="3">
         <v>1</v>
       </c>
-      <c r="D40" s="7">
-        <v>2</v>
-      </c>
-      <c r="E40" s="3">
+      <c r="D40" s="8">
+        <v>2</v>
+      </c>
+      <c r="E40" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1298,12 +1304,16 @@
       <c r="C41" s="3">
         <v>2</v>
       </c>
-      <c r="D41" s="3">
-        <v>5</v>
-      </c>
-      <c r="E41" s="3">
-        <v>4</v>
-      </c>
+      <c r="D41" s="8">
+        <v>5</v>
+      </c>
+      <c r="E41" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Update a_psat model manager, urls, views, admin_psat_utils, templates
</commit_message>
<xml_diff>
--- a/a_psat/data/answer_official.xlsx
+++ b/a_psat/data/answer_official.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\paedison3\a_psat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3E5725-2294-46AC-B851-64955CBC5E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C58B75E-CBB0-408F-87BA-6B19EC9F6381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27525" yWindow="9270" windowWidth="19080" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-54720" yWindow="2220" windowWidth="16440" windowHeight="28440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="정답" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -634,9 +647,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
@@ -872,7 +883,7 @@
       <c r="B14" s="3">
         <v>4</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="8">
         <v>4</v>
       </c>
       <c r="D14" s="3">
@@ -1154,7 +1165,7 @@
       <c r="C31" s="3">
         <v>3</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <v>5</v>
       </c>
       <c r="E31" s="8">

</xml_diff>